<commit_message>
Pruebas unitarias para ciclo 2
</commit_message>
<xml_diff>
--- a/NoteBook/test plans and data/Plan de Pruebas Unitarias.xlsx
+++ b/NoteBook/test plans and data/Plan de Pruebas Unitarias.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -370,6 +370,287 @@
   </si>
   <si>
     <t>Éxito: La cadena que retorna el método coincide con los cambios realizados en ambas versiones</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar el correcto funcionamiento del método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"crearCarpeta" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de la clase UtilidadesArchivo.java</t>
+    </r>
+  </si>
+  <si>
+    <t>ruta="D:\\PruebasCrearCarpeta"</t>
+  </si>
+  <si>
+    <t>Verificar que el método crea la carpeta en la ruta indicada</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar correcto manejo de errores del método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"crearCarpeta" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de la clase UtilidadesArchivo.java</t>
+    </r>
+  </si>
+  <si>
+    <t>Verificar que el método maneje los errores cuando los parámetros no se envían correctamente</t>
+  </si>
+  <si>
+    <t>Éxito: la carpeta se crea en la ruta indicada</t>
+  </si>
+  <si>
+    <t>ruta="/**/)"</t>
+  </si>
+  <si>
+    <t>Éxito: la carpeta no es creada y el método retorna false</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar el correcto funcionamiento del método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"crearArchivo" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de la clase UtilidadesArchivo.java</t>
+    </r>
+  </si>
+  <si>
+    <t>Verificar que el método cree el archivo en la ruta indicada</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar correcto manejo de errores del método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"crearArchivo" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de la clase UtilidadesArchivo.java</t>
+    </r>
+  </si>
+  <si>
+    <t>rutaArchivo="D:\\PruebasCrearCarpeta\\pruebaarchivo.java"</t>
+  </si>
+  <si>
+    <t>rutaArchivo="D:\\CarpetaInexistente\\archivo.java"</t>
+  </si>
+  <si>
+    <t>Verificar que el método maneje los errores cuando la carpeta no existe en el sistema</t>
+  </si>
+  <si>
+    <t>Éxito: el archivo se crea correctamente</t>
+  </si>
+  <si>
+    <t>Éxito: se captura la excepción se muestra mensaje en log y se retorna false indicando que no se creó el archivo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar que el método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"escribirNuevaLineaEnArchivo" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de la clase UtilidadesArchivo.java ingrese una nueva línea en el archivo enviado como parámetro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar que el método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"leerLineasArchivo"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de la clase UtilidadesArchivo.java obtenga todas las lineas del archivo enviada como parámetro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar que el método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"copiarCarpeta"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de la clase UtilidadesArchivo.java realice la copia de la carpeta enviada como parámetro a la ruta destino enviada como parámetro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar que el método </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"copyFile"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de la clase UtilidadesArchivo.java realice la copia un archivo de origen y destino enviados como parámetro</t>
+    </r>
+  </si>
+  <si>
+    <t>rutaArchivo = "D:\\PruebasCarpetaOrigen\\Prueba.java", nuevaLinea = "primera linea"</t>
+  </si>
+  <si>
+    <t>rutaArchivo = "D:\\PruebasCarpetaOrigen\\Prueba.java", ArrayList expResult = new ArrayList(); expResult.add("primera linea");</t>
+  </si>
+  <si>
+    <t>carpetaOrigen = "D:\\PruebasCarpetaOrigen";carpetaDestino = "D:\\PruebasCopia";</t>
+  </si>
+  <si>
+    <t>Verificar que se creó la nueva línea en el archivo enviado como parámetro</t>
+  </si>
+  <si>
+    <t>Verificar que las lineas coincidan con las del archivo enviado</t>
+  </si>
+  <si>
+    <t>Verificar que la carpeta copiada se encuentre en la nueva ruta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar que la copia del archivo se encuentre en la ruta destino </t>
+  </si>
+  <si>
+    <t>File s = new File("D:\\PruebasCarpetaOrigen\\Prueba.java");
+File t = new File("D:\\PruebasCarpetaOrigen\\Prueba2.java");</t>
+  </si>
+  <si>
+    <t>Éxito: la linea se agrega correctamente al archivo</t>
+  </si>
+  <si>
+    <t>Éxito: las lineas obtenidas coinciden con las que tiene el archivo</t>
+  </si>
+  <si>
+    <t>Éxito: el contenido de la carpeta origen es copiado a la carpeta destino</t>
+  </si>
+  <si>
+    <t>Éxito: El archivo es copiado al archivo destino correctamente</t>
   </si>
 </sst>
 </file>
@@ -415,9 +696,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,6 +711,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,233 +1035,349 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>